<commit_message>
Version EEE with web build for IOS
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="6780"/>
+    <workbookView windowWidth="20490" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$D$1:$D$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$C$1:$C$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -146,13 +146,13 @@
     <t>LVSI+</t>
   </si>
   <si>
+    <t>Stage IIC-cervical stroma +</t>
+  </si>
+  <si>
+    <t>VBT/observation</t>
+  </si>
+  <si>
     <t>Any</t>
-  </si>
-  <si>
-    <t>Stage IIC-cervical stroma +</t>
-  </si>
-  <si>
-    <t>VBT/observation</t>
   </si>
   <si>
     <t>High (G3)</t>
@@ -252,13 +252,19 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -725,138 +731,141 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1395,7 +1404,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -2062,14 +2071,14 @@
       <c r="B26" t="s">
         <v>37</v>
       </c>
-      <c r="C26" t="s">
-        <v>38</v>
+      <c r="C26" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D26" t="s">
         <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F26" t="s">
         <v>30</v>
@@ -2088,8 +2097,8 @@
       <c r="B27" t="s">
         <v>37</v>
       </c>
-      <c r="C27" t="s">
-        <v>38</v>
+      <c r="C27" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
@@ -2156,7 +2165,7 @@
         <v>31</v>
       </c>
       <c r="H29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2164,7 +2173,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
         <v>41</v>
@@ -2190,7 +2199,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
         <v>41</v>
@@ -2216,7 +2225,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
         <v>41</v>
@@ -2242,7 +2251,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
         <v>41</v>
@@ -2268,7 +2277,7 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
         <v>41</v>
@@ -2294,7 +2303,7 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
         <v>41</v>
@@ -2320,7 +2329,7 @@
         <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
         <v>41</v>
@@ -2346,7 +2355,7 @@
         <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
         <v>41</v>
@@ -2372,7 +2381,7 @@
         <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
         <v>41</v>
@@ -2398,7 +2407,7 @@
         <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
         <v>41</v>
@@ -2424,7 +2433,7 @@
         <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
         <v>41</v>
@@ -2450,7 +2459,7 @@
         <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
         <v>41</v>
@@ -2476,13 +2485,13 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E42" t="s">
         <v>50</v>
@@ -2502,10 +2511,10 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D43" t="s">
         <v>51</v>
@@ -2528,13 +2537,13 @@
         <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E44" t="s">
         <v>50</v>
@@ -2554,10 +2563,10 @@
         <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D45" t="s">
         <v>51</v>
@@ -2577,13 +2586,13 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D46" t="s">
         <v>18</v>
@@ -2918,10 +2927,10 @@
         <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
-      </c>
-      <c r="C59" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -2944,10 +2953,10 @@
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
-      </c>
-      <c r="C60" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
@@ -2970,13 +2979,13 @@
         <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>38</v>
-      </c>
-      <c r="C61" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E61" t="s">
         <v>60</v>
@@ -2996,13 +3005,13 @@
         <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>38</v>
-      </c>
-      <c r="C62" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E62" t="s">
         <v>64</v>
@@ -3022,13 +3031,13 @@
         <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>38</v>
-      </c>
-      <c r="C63" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E63" t="s">
         <v>65</v>
@@ -3048,13 +3057,13 @@
         <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
-      </c>
-      <c r="C64" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E64" t="s">
         <v>66</v>
@@ -3074,13 +3083,13 @@
         <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>38</v>
-      </c>
-      <c r="C65" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E65" t="s">
         <v>67</v>
@@ -3100,13 +3109,13 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>38</v>
-      </c>
-      <c r="C66" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E66" t="s">
         <v>60</v>
@@ -3126,13 +3135,13 @@
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
-      </c>
-      <c r="C67" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E67" t="s">
         <v>64</v>
@@ -3152,13 +3161,13 @@
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>38</v>
-      </c>
-      <c r="C68" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D68" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E68" t="s">
         <v>68</v>
@@ -3178,13 +3187,13 @@
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>38</v>
-      </c>
-      <c r="C69" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E69" t="s">
         <v>69</v>
@@ -3204,13 +3213,13 @@
         <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>38</v>
-      </c>
-      <c r="C70" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D70" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E70" t="s">
         <v>67</v>
@@ -3226,7 +3235,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="D1:D70" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="C1:C70" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>